<commit_message>
add new function: order constraint checking
</commit_message>
<xml_diff>
--- a/template/activity_order.xlsx
+++ b/template/activity_order.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20374"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04842027-99F8-4914-8ADB-542ED07D1F96}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950E5D0B-E3FB-4EB7-A2A7-1E88E502E2E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="169">
   <si>
     <t>T10010</t>
   </si>
@@ -625,7 +625,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -635,6 +635,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -916,10 +919,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B220"/>
+  <dimension ref="A1:B221"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1192,19 +1195,19 @@
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="1" t="s">
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A35" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A35" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.4">
@@ -1212,15 +1215,15 @@
         <v>42</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.4">
@@ -1228,7 +1231,7 @@
         <v>35</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.4">
@@ -1236,7 +1239,7 @@
         <v>35</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.4">
@@ -1244,7 +1247,7 @@
         <v>35</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.4">
@@ -1252,7 +1255,7 @@
         <v>35</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.4">
@@ -1260,39 +1263,39 @@
         <v>35</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A43" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A45" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A46" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.4">
@@ -1300,23 +1303,23 @@
         <v>51</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A48" s="1" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A49" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.4">
@@ -1324,7 +1327,7 @@
         <v>54</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.4">
@@ -1332,15 +1335,15 @@
         <v>54</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A52" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.4">
@@ -1348,39 +1351,39 @@
         <v>55</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A54" s="1" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A55" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A56" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A57" s="1" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.4">
@@ -1388,7 +1391,7 @@
         <v>40</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.4">
@@ -1396,12 +1399,12 @@
         <v>40</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A60" s="1" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>64</v>
@@ -1409,10 +1412,10 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A61" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.4">
@@ -1420,15 +1423,15 @@
         <v>64</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A63" s="1" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.4">
@@ -1436,23 +1439,23 @@
         <v>44</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A65" s="1" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A66" s="1" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>67</v>
+        <v>19</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.4">
@@ -1460,7 +1463,7 @@
         <v>45</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.4">
@@ -1468,63 +1471,63 @@
         <v>45</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A69" s="1" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A70" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>68</v>
+        <v>18</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A71" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A72" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A73" s="1" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>70</v>
+        <v>19</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A74" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A75" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.4">
@@ -1532,7 +1535,7 @@
         <v>71</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.4">
@@ -1540,31 +1543,31 @@
         <v>71</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A78" s="1" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A79" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A80" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.4">
@@ -1572,15 +1575,15 @@
         <v>74</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A82" s="1" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.4">
@@ -1588,23 +1591,23 @@
         <v>53</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A84" s="1" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A85" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B85" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.4">
@@ -1612,7 +1615,7 @@
         <v>76</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.4">
@@ -1620,23 +1623,23 @@
         <v>76</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A88" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A89" s="1" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>78</v>
+        <v>19</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.4">
@@ -1644,7 +1647,7 @@
         <v>61</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.4">
@@ -1652,31 +1655,31 @@
         <v>61</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A92" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>79</v>
+        <v>27</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A93" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B93" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A94" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B94" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.4">
@@ -1684,23 +1687,23 @@
         <v>80</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A96" s="1" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A97" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.4">
@@ -1708,31 +1711,31 @@
         <v>57</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A99" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A100" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A101" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B101" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.4">
@@ -1740,39 +1743,39 @@
         <v>84</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A103" s="1" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>82</v>
+        <v>19</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A104" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B104" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A105" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A106" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B106" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.4">
@@ -1780,79 +1783,79 @@
         <v>81</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A108" s="1" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A109" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B109" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A110" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B110" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A111" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B111" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A112" s="1" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>91</v>
+        <v>18</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A113" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B113" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A114" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B114" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A115" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B115" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A116" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B116" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.4">
@@ -1860,7 +1863,7 @@
         <v>93</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.4">
@@ -1868,15 +1871,15 @@
         <v>93</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A119" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.4">
@@ -1884,15 +1887,15 @@
         <v>87</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>94</v>
+        <v>27</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A121" s="1" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>27</v>
+        <v>94</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.4">
@@ -1900,15 +1903,15 @@
         <v>26</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A123" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.4">
@@ -1916,39 +1919,39 @@
         <v>27</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A125" s="1" t="s">
-        <v>94</v>
+        <v>27</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A126" s="1" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A127" s="1" t="s">
-        <v>18</v>
+        <v>86</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A128" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.4">
@@ -1956,87 +1959,87 @@
         <v>19</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A130" s="1" t="s">
-        <v>95</v>
+        <v>19</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>96</v>
+        <v>18</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A131" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B131" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="B131" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A132" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B132" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A133" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B133" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="B133" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A134" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A135" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B135" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="B135" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A136" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B136" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="B136" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A137" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B137" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="B137" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A138" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B138" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="B138" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A139" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B139" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="B139" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.4">
@@ -2044,15 +2047,15 @@
         <v>105</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A141" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.4">
@@ -2060,15 +2063,15 @@
         <v>106</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A143" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.4">
@@ -2076,199 +2079,199 @@
         <v>108</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A145" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>0</v>
+        <v>107</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A146" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>112</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A147" s="1" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A148" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B148" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="B148" s="1" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A149" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B149" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="B149" s="1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A150" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B150" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="B150" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A151" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B151" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="B151" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A152" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B152" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A153" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B153" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A154" s="1" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A155" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B155" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="B155" s="1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A156" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B156" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="B156" s="1" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A157" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B157" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A158" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B158" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="B158" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A159" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B159" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="B159" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A160" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B160" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="B160" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A161" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B161" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="B161" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A162" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B162" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="B162" s="1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A163" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B163" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="B163" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A164" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B164" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="B164" s="1" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A165" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B165" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="B165" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A166" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B166" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A167" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B167" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="B167" s="1" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A168" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B168" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="B168" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.4">
@@ -2276,7 +2279,7 @@
         <v>132</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.4">
@@ -2284,7 +2287,7 @@
         <v>132</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.4">
@@ -2292,7 +2295,7 @@
         <v>132</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.4">
@@ -2300,7 +2303,7 @@
         <v>132</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>111</v>
+        <v>46</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.4">
@@ -2308,364 +2311,364 @@
         <v>132</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A174" s="1" t="s">
-        <v>0</v>
+        <v>132</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>1</v>
+        <v>133</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A175" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B175" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="B175" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A176" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B176" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B176" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A177" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B177" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B177" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A178" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B178" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B178" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A179" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B179" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B179" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A180" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B180" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B180" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A181" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B181" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B181" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A182" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B182" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B182" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A183" s="1" t="s">
-        <v>107</v>
+        <v>8</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A184" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B184" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="B184" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A185" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B185" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="B185" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A186" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B186" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="B186" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A187" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B187" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="B187" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A188" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B188" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="B188" s="1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A189" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B189" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="B189" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A190" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B190" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="B190" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A191" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B191" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="B191" s="1" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A192" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B192" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="B192" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A193" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B193" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="B193" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A194" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B194" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="B194" s="1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A195" s="1" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A196" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B196" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="B196" s="1" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A197" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B197" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="B197" s="1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A198" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B198" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="B198" s="1" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A199" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B199" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="B199" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A200" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B200" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="B200" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A201" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B201" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="B201" s="1" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A202" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B202" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="B202" s="1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A203" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B203" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="B203" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A204" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B204" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="B204" s="1" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A205" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B205" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="B205" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A206" s="1" t="s">
-        <v>134</v>
+        <v>156</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>157</v>
+        <v>112</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A207" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B207" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="B207" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A208" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B208" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="B208" s="1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A209" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B209" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="B209" s="1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A210" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B210" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="B210" s="1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A211" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B211" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="B211" s="1" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A212" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B212" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="B212" s="1" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A213" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B213" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="B213" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A214" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B214" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="B214" s="1" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A215" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B215" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="B215" s="1" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A216" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B216" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="B216" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A217" s="1" t="s">
-        <v>112</v>
+        <v>166</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>167</v>
+        <v>95</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A218" s="1" t="s">
-        <v>146</v>
+        <v>112</v>
       </c>
       <c r="B218" s="1" t="s">
         <v>167</v>
@@ -2673,17 +2676,25 @@
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A219" s="1" t="s">
-        <v>62</v>
+        <v>146</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A220" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A221" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B220" s="1" t="s">
+      <c r="B221" s="1" t="s">
         <v>167</v>
       </c>
     </row>

</xml_diff>